<commit_message>
Selection of GD, BUCK and LDO
</commit_message>
<xml_diff>
--- a/hardware/Component-Library.xlsx
+++ b/hardware/Component-Library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\binon\Desktop\Kururugi-ESC-Dev-Board\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F16D14-A130-4E4B-89F9-D81E29395C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5018C17-9BAA-4910-868C-6BE8B8102378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,17 +18,28 @@
     <sheet name="Interfaces" sheetId="2" r:id="rId3"/>
     <sheet name="Draft" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="242">
   <si>
     <t>Category</t>
   </si>
@@ -698,12 +709,6 @@
     <t>Search for buck</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/filter/voltage-regulators-dc-dc-switching-regulators/739?s=N4IgjCBcoBwOxVAYygMwIYBsDOBTANCAPZQDa4ATGAMwUBsIhALAAwXUyMjUCcddAVhABdQgAcALlBABlCQCcAlgDsA5iAC%2BhMGBaIQKSBhwFiZEKxjUWnUSEnS5StZu0Ue%2Bw8byESkcuwUMHQIhPR09BBh-NRwUSDhvBRc4UxgQmEC7hEpAkxMFBkJMCxwNik8sRRMFRx0nGFWlTWE1kwwPB6EcNVpXHDUYHTU-TzBoSDBMPRc0yxMRXz88bqFOly6cHTtG%2BkwMC3gBfNdRx3DG3lMsZdWF9oCB0wM2sPpyXYOkLIKKupaIAEA08aCwPjM-gSQO2yWi1jGKTgaV0KXgwwm1V4AgYnyk3ycf1cR3cIKMYNMfnI8DiDRASIE6VmLEGRTgAgZLzpdBY236MNOWy2RWmkVm1Top2m%2B3iVjYMvcO0IPEKJMI%2B0GsMmwUVWpKnI6YDgEw6eU1Jp6sx4j0OPCRzP66VtE0qmy4zQ6buo1z0SuoEp9IEq7MWvCYztY8zdrGqG2ZprdVjAtLGaU5KYlCbiNvg7DdPBsmt08AKsYKwVL105unaC1LnQmuiyDN29BYRV0QdOHeeKxYYwEI20uiGtJ0gj7u2oHFHNBCAZ0sXZu1tht2cQo88NFDgXa3rDXA-bhp6g-Ax%2Bea7ZXeuJVPNH2dBW06CG14NHnST62meHK49UfIQbPkj7XmG1hAWGMArEwPDXIcYBhn2DZhuw7ZhnBlxJgi362iWOFopcLAsGAXYCHKo5kbQKzskmd5NgclyFI%2BlzKmGlyPPwlwRDkrwIauDxWmxAlsoWAidC%2BrxenEGyPiKMkblaMkcYWwx3DJEZdtsCENvwFASeA-DtO2BxiaOUG0FW2ootoBx8F2%2BxQfZ-DNjZISAa5JROfAKzwG2hb5gy84dPMQUuqFfqFh0aTwcqxHtvmWyHAcCn%2BTWMXsERGy2rE85jDuVa2nOWVwNKKREVQ-n5vkWU8LouW1eU2idEmtIbnsmobm2bBlTy1kJOk1hFFQA6Nf1VAMWEYDsFNKRDNirXpGRAbDcMHXpI%2BhwrZUs1AkCs16hMAz5vsf4hNinLjdUrJDBEQ16VO8T3QsGJXSdYSRDG73bGJKQcAMrXUGJzFhLwUFDZYWS-eJF1pHKKQFGJGLXFaMPbryYRlvU8OPlO8NZIpGMDmyeMFI9zzNf0QJ1djfqtWGEqnNUcT2pkiUdY8vCnO0JQzdEBabdyVUpMMfa0s8ba8MLrBkVLbKntuyLLWyzmIqtAZhgyuNhCVSYXSVMAucUWw3GEtWVhUzUTNYuiDH%2BfCqnSNDXLMZanLBbKjkRIQQLiji-C4AIkR60AGKCJi%2BOYejCACAC0yQh4YCgAK4UuYQjRwCDAh4oAAm0gx8OXBfCAXASAAnmIuDSOg2AoBoGhAA</t>
-  </si>
-  <si>
-    <t>In 17V, Out 3A</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/vishay-siliconix/SIC472ED-T1-GE3/9556546</t>
   </si>
   <si>
@@ -717,6 +722,51 @@
   </si>
   <si>
     <t>ICs</t>
+  </si>
+  <si>
+    <t>https://www.monolithicpower.com/en/documentview/productdocument/index/version/2/document_type/Datasheet/lang/en/sku/MP4436AGR/document_id/8690/</t>
+  </si>
+  <si>
+    <t>GATE DRIVER</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/en/products/detail/infineon-technologies/2EDL8024GXUMA1/13582321</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/en/products/detail/monolithic-power-systems-inc/MP1922GV-Z/16579179</t>
+  </si>
+  <si>
+    <t>MP1922</t>
+  </si>
+  <si>
+    <t>22-QFN</t>
+  </si>
+  <si>
+    <t>to 100Vin, to 15Vgate, 3A source, 4A sink</t>
+  </si>
+  <si>
+    <t>to 100Vin, to 17Vgate, 4A source, 6A sink HS, 5A sink LS</t>
+  </si>
+  <si>
+    <t>2EDL8024G3C</t>
+  </si>
+  <si>
+    <t>2EDL8024G</t>
+  </si>
+  <si>
+    <t>VDSON-8-4 (4x4mm)</t>
+  </si>
+  <si>
+    <t>VDSON-10-4 (3x3mm)</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/InfineonTechnologies-2EDL8024G/C3655215</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/voltage-regulators-dc-dc-switching-regulators/739?s=N4IgjCBcoGwJxVAYygMwIYBsDOBTANCAPZQDaIALAAxwUDMVIh1cdrIAuoQA4AuUIAMq8ATgEsAdgHMQAX0IAOAOyIQKSBhwFiZcACYwdPTCaUqeugtNsYMAKyce-SENGSZ88GEbQ1aLHiEJJDk1AoMVlwgfALC4tJyhGB6CL7qmoE6ISB6VGB2tKaG%2BXQQSTBKBRSmBRZ0NXZUFBBRMS5x7ok5dg5p-lpBupZweQiEw02Mrc6u8R6Edkr1fRoB2sHkelt0paZ69HB2JoR6izAUenswDHBWJ0rN3nvK1yrTsW4Jnoa5qulrg2yFx2KUc0RmHS%2BSVuqWQ-UyGxAU08AFpLitRABXda6BwcWSeEy%2BMQAEwEKO8ZXBAlMvAAntxcAJ0NgUASgA</t>
+  </si>
+  <si>
+    <t>In 17V, Out 0.9-6V@3A</t>
   </si>
 </sst>
 </file>
@@ -802,7 +852,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -918,134 +968,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1055,7 +985,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1099,6 +1029,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1108,12 +1056,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1129,94 +1077,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1507,15 +1381,16 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="B1:K26"/>
+  <dimension ref="B2:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" customWidth="1"/>
     <col min="3" max="3" width="23.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.26953125" style="2" customWidth="1"/>
@@ -1524,84 +1399,83 @@
     <col min="8" max="8" width="21.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:11" ht="26" x14ac:dyDescent="0.6">
-      <c r="B2" s="40" t="s">
-        <v>228</v>
-      </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B3" s="43" t="s">
+    <row r="2" spans="2:10" ht="26" x14ac:dyDescent="0.6">
+      <c r="B2" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="34" t="s">
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="34" t="s">
-        <v>226</v>
-      </c>
-      <c r="J3" s="44"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B4" s="43"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="36" t="s">
+      <c r="H3" s="36"/>
+      <c r="I3" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="J3" s="36"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="37" t="s">
+      <c r="I4" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="J4" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="J4" s="45" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B5" s="46" t="s">
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="47"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B6" s="48" t="s">
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -1622,13 +1496,13 @@
       <c r="I6" s="9">
         <v>0</v>
       </c>
-      <c r="J6" s="56">
+      <c r="J6" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="B7" s="48"/>
-      <c r="C7" s="59" t="s">
+    <row r="7" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B7" s="25"/>
+      <c r="C7" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1647,13 +1521,13 @@
       <c r="I7" s="9">
         <v>0</v>
       </c>
-      <c r="J7" s="56">
+      <c r="J7" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="B8" s="48"/>
-      <c r="C8" s="59" t="s">
+    <row r="8" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B8" s="25"/>
+      <c r="C8" s="21" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -1674,15 +1548,15 @@
       <c r="I8" s="9">
         <v>0</v>
       </c>
-      <c r="J8" s="56">
+      <c r="J8" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B9" s="48" t="s">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="21" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -1703,13 +1577,13 @@
       <c r="I9" s="9">
         <v>0</v>
       </c>
-      <c r="J9" s="56">
+      <c r="J9" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B10" s="48"/>
-      <c r="C10" s="59" t="s">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="25"/>
+      <c r="C10" s="21" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -1726,15 +1600,15 @@
       <c r="I10" s="9">
         <v>0</v>
       </c>
-      <c r="J10" s="56">
+      <c r="J10" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B11" s="48" t="s">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="21" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -1751,13 +1625,13 @@
       <c r="I11" s="9">
         <v>0</v>
       </c>
-      <c r="J11" s="56">
+      <c r="J11" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B12" s="48"/>
-      <c r="C12" s="59" t="s">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="25"/>
+      <c r="C12" s="21" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -1778,25 +1652,25 @@
       <c r="I12" s="9">
         <v>0</v>
       </c>
-      <c r="J12" s="56">
+      <c r="J12" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B13" s="49" t="s">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="50"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B14" s="48" t="s">
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1820,12 +1694,12 @@
       <c r="I14" s="9">
         <v>0</v>
       </c>
-      <c r="J14" s="56">
+      <c r="J14" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B15" s="48"/>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="25"/>
       <c r="C15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1837,13 +1711,12 @@
       <c r="I15" s="9">
         <v>0</v>
       </c>
-      <c r="J15" s="56">
+      <c r="J15" s="9">
         <v>1</v>
       </c>
-      <c r="K15" s="29"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B16" s="48"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="25"/>
       <c r="C16" s="4" t="s">
         <v>20</v>
       </c>
@@ -1857,25 +1730,25 @@
       <c r="I16" s="9">
         <v>0</v>
       </c>
-      <c r="J16" s="56">
+      <c r="J16" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="50"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1897,12 +1770,12 @@
       <c r="I18" s="9">
         <v>0</v>
       </c>
-      <c r="J18" s="56">
+      <c r="J18" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="25" t="s">
         <v>180</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1926,12 +1799,12 @@
       <c r="I19" s="9">
         <v>0</v>
       </c>
-      <c r="J19" s="56">
+      <c r="J19" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B20" s="48"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="4" t="s">
         <v>184</v>
       </c>
@@ -1951,12 +1824,12 @@
       <c r="I20" s="9">
         <v>0</v>
       </c>
-      <c r="J20" s="56">
+      <c r="J20" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="48"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="4" t="s">
         <v>181</v>
       </c>
@@ -1974,12 +1847,12 @@
       <c r="I21" s="9">
         <v>0</v>
       </c>
-      <c r="J21" s="56">
+      <c r="J21" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="37" t="s">
         <v>61</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -1992,7 +1865,7 @@
         <v>136</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>167</v>
@@ -2003,98 +1876,191 @@
       <c r="I22" s="9">
         <v>0</v>
       </c>
-      <c r="J22" s="56">
+      <c r="J22" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B23" s="48"/>
+      <c r="B23" s="38"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="7"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I23" s="9">
         <v>0</v>
       </c>
-      <c r="J23" s="56">
+      <c r="J23" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B24" s="49" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="50"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="I24" s="9">
+        <v>0</v>
+      </c>
+      <c r="J24" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B25" s="48" t="s">
-        <v>119</v>
+      <c r="B25" s="37" t="s">
+        <v>228</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>120</v>
+        <v>231</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>137</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="E25" s="7"/>
       <c r="F25" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>122</v>
+        <v>233</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4" t="s">
+        <v>230</v>
       </c>
       <c r="I25" s="9">
         <v>0</v>
       </c>
-      <c r="J25" s="56">
+      <c r="J25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B26" s="38"/>
+      <c r="C26" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="I26" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="52"/>
-      <c r="C26" s="53" t="s">
+      <c r="J26" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B27" s="39"/>
+      <c r="C27" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="I27" s="9">
+        <v>1</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B28" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B29" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I29" s="9">
+        <v>0</v>
+      </c>
+      <c r="J29" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B30" s="25"/>
+      <c r="C30" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D26" s="53" t="s">
+      <c r="D30" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E26" s="54"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="55" t="s">
+      <c r="E30" s="7"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="I26" s="57">
+      <c r="I30" s="9">
         <v>0</v>
       </c>
-      <c r="J26" s="58">
+      <c r="J30" s="9">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
+    <mergeCell ref="B5:J5"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="B28:J28"/>
     <mergeCell ref="B17:J17"/>
     <mergeCell ref="B13:J13"/>
-    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B29:B30"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
@@ -2104,11 +2070,9 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B2:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="I6:J12">
-    <cfRule type="iconSet" priority="16">
+    <cfRule type="iconSet" priority="37">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="1"/>
@@ -2117,7 +2081,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:J16">
-    <cfRule type="iconSet" priority="3">
+    <cfRule type="iconSet" priority="24">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="1"/>
@@ -2125,8 +2089,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18:J23">
-    <cfRule type="iconSet" priority="2">
+  <conditionalFormatting sqref="I18:J27">
+    <cfRule type="iconSet" priority="23">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="1"/>
@@ -2134,8 +2098,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I25:J26">
-    <cfRule type="iconSet" priority="1">
+  <conditionalFormatting sqref="I29:J30">
+    <cfRule type="iconSet" priority="22">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0" gte="0"/>
@@ -2156,10 +2120,10 @@
     <hyperlink ref="E18" r:id="rId10" xr:uid="{BF3C2DEE-319B-47CA-BB7F-CC9DDD316D83}"/>
     <hyperlink ref="H22" r:id="rId11" xr:uid="{D8A1F51B-D01B-44C7-9E49-7FA996B83847}"/>
     <hyperlink ref="E22" r:id="rId12" xr:uid="{8D02B26B-9403-49DB-A3FC-4974493D9149}"/>
-    <hyperlink ref="H25" r:id="rId13" xr:uid="{78BFE1A1-9DCE-412E-BEF0-1F3E51F9DC44}"/>
-    <hyperlink ref="E25" r:id="rId14" xr:uid="{FF2076C3-F5D2-4C97-8BCA-B03FB41885C8}"/>
-    <hyperlink ref="G25" r:id="rId15" xr:uid="{95E773F7-E1C0-4DC2-8D2F-7AD94AA9D51B}"/>
-    <hyperlink ref="H26" r:id="rId16" xr:uid="{84B931C7-29AD-4AB1-87E2-CD8764EDB628}"/>
+    <hyperlink ref="H29" r:id="rId13" xr:uid="{78BFE1A1-9DCE-412E-BEF0-1F3E51F9DC44}"/>
+    <hyperlink ref="E29" r:id="rId14" xr:uid="{FF2076C3-F5D2-4C97-8BCA-B03FB41885C8}"/>
+    <hyperlink ref="G29" r:id="rId15" xr:uid="{95E773F7-E1C0-4DC2-8D2F-7AD94AA9D51B}"/>
+    <hyperlink ref="H30" r:id="rId16" xr:uid="{84B931C7-29AD-4AB1-87E2-CD8764EDB628}"/>
     <hyperlink ref="G22" r:id="rId17" xr:uid="{8FDCAB0A-B033-4912-B883-1EDAC34E8B2D}"/>
     <hyperlink ref="H6" r:id="rId18" xr:uid="{D276D29E-36B9-4147-86FC-A90EAC58CC7A}"/>
     <hyperlink ref="G6" r:id="rId19" xr:uid="{EFCE5A43-584C-4B82-AD48-0B1F2ADEDA83}"/>
@@ -2209,25 +2173,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="20" t="s">
+      <c r="E2" s="28"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="21"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
       <c r="D3" s="16" t="s">
         <v>32</v>
       </c>
@@ -2245,7 +2209,7 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="25" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -2268,7 +2232,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B5" s="19"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="4" t="s">
         <v>41</v>
       </c>
@@ -2287,7 +2251,7 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B6" s="19"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="4" t="s">
         <v>45</v>
       </c>
@@ -2308,7 +2272,7 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="19"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="4" t="s">
         <v>49</v>
       </c>
@@ -2350,7 +2314,7 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="25" t="s">
         <v>81</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -2373,7 +2337,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="19"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="4" t="s">
         <v>86</v>
       </c>
@@ -2394,7 +2358,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="25" t="s">
         <v>90</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -2413,7 +2377,7 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="19"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="4"/>
       <c r="D12" s="10" t="s">
         <v>91</v>
@@ -2426,7 +2390,7 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="19"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="4"/>
       <c r="D13" s="10" t="s">
         <v>92</v>
@@ -2439,7 +2403,7 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="19"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="4" t="s">
         <v>195</v>
       </c>
@@ -2458,7 +2422,7 @@
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="19"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="4" t="s">
         <v>200</v>
       </c>
@@ -2500,7 +2464,7 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="25" t="s">
         <v>101</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -2523,7 +2487,7 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B18" s="19"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="4" t="s">
         <v>102</v>
       </c>
@@ -2544,7 +2508,7 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B19" s="19"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="4" t="s">
         <v>107</v>
       </c>
@@ -2588,7 +2552,7 @@
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="25" t="s">
         <v>150</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -2609,7 +2573,7 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B22" s="19"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="4" t="s">
         <v>156</v>
       </c>
@@ -2736,25 +2700,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="20" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="21"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="17" t="s">
         <v>32</v>
       </c>
@@ -2816,7 +2780,7 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="25" t="s">
         <v>71</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -2837,7 +2801,7 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B7" s="19"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="4" t="s">
         <v>74</v>
       </c>
@@ -2856,7 +2820,7 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B8" s="19"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="4" t="s">
         <v>78</v>
       </c>
@@ -2875,7 +2839,7 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B9" s="19"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="4" t="s">
         <v>97</v>
       </c>
@@ -2933,7 +2897,7 @@
   <dimension ref="B2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2948,7 +2912,7 @@
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>222</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>